<commit_message>
pengujian menu dan search sukses
</commit_message>
<xml_diff>
--- a/laporan_testing_search.xlsx
+++ b/laporan_testing_search.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>hasil_screenshot\screenshot_025729.png</t>
+          <t>hasil_screenshot\screenshot_095849.png</t>
         </is>
       </c>
     </row>
@@ -468,7 +468,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>hasil_screenshot\screenshot_025733.png</t>
+          <t>hasil_screenshot\screenshot_095852.png</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>hasil_screenshot\screenshot_025734.png</t>
+          <t>hasil_screenshot\screenshot_095854.png</t>
         </is>
       </c>
     </row>
@@ -502,7 +502,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>hasil_screenshot\screenshot_025737.png</t>
+          <t>hasil_screenshot\screenshot_095856.png</t>
         </is>
       </c>
     </row>

</xml_diff>